<commit_message>
Renaming, and potentially starting the great BR Mk 1 modularization
</commit_message>
<xml_diff>
--- a/docs/Cost Factor Calculator.xlsx
+++ b/docs/Cost Factor Calculator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BRTrains2-Extended\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C28CB5C0-F079-4C88-82C9-2B02FDF80F42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61F5B18B-85F1-42B0-B9E6-E9BA49798AE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cost Factor Calculator" sheetId="1" r:id="rId1"/>
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2857" uniqueCount="1088">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2859" uniqueCount="1088">
   <si>
     <t>ITEM_NAME</t>
   </si>
@@ -3556,7 +3556,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3676,6 +3676,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -4671,10 +4677,10 @@
   <dimension ref="A1:X885"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D286" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D245" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J304" sqref="J304"/>
+      <selection pane="bottomRight" activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6450,21 +6456,27 @@
       <c r="I25" s="1">
         <v>1</v>
       </c>
+      <c r="L25" s="6" t="s">
+        <v>342</v>
+      </c>
+      <c r="M25" s="6" t="s">
+        <v>342</v>
+      </c>
       <c r="N25" s="1" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="T25" s="1" t="str">
+      <c r="T25" s="1">
         <f t="shared" si="7"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="U25" s="14" t="e">
         <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
-      <c r="V25" s="14" t="str">
+      <c r="V25" s="14" t="e">
         <f t="shared" si="3"/>
-        <v/>
+        <v>#VALUE!</v>
       </c>
       <c r="W25" s="20" t="e">
         <f t="shared" si="4"/>
@@ -7995,81 +8007,82 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="48" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A48" s="21">
+    <row r="48" spans="1:24" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="41">
         <v>724</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B48" s="9" t="s">
         <v>572</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="C48" s="9" t="s">
         <v>679</v>
       </c>
-      <c r="D48" s="1" t="str">
+      <c r="D48" s="9" t="str">
         <f t="shared" si="8"/>
         <v>BR</v>
       </c>
-      <c r="E48" s="1" t="s">
+      <c r="E48" s="9" t="s">
         <v>360</v>
       </c>
-      <c r="F48" s="1">
+      <c r="F48" s="9">
         <v>1951</v>
       </c>
-      <c r="G48" s="1" t="s">
+      <c r="G48" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="H48" s="18">
+      <c r="H48" s="42">
         <f t="shared" si="9"/>
         <v>11.090536506409418</v>
       </c>
-      <c r="I48" s="1">
+      <c r="I48" s="9">
         <v>1</v>
       </c>
-      <c r="J48" s="1">
+      <c r="J48" s="9">
         <v>32</v>
       </c>
-      <c r="K48" s="1">
+      <c r="K48" s="9">
         <v>64</v>
       </c>
-      <c r="L48" s="6" t="s">
+      <c r="L48" s="9" t="s">
         <v>342</v>
       </c>
-      <c r="M48" s="6" t="s">
+      <c r="M48" s="9" t="s">
         <v>342</v>
       </c>
-      <c r="N48" s="1" t="str">
+      <c r="N48" s="9" t="str">
         <f>IF(L48="Steam",1,IF(L48="Electric",2,IF(L48="Diesel",4,IF(L48="Diesel-Electric",3,""))))</f>
         <v/>
       </c>
-      <c r="O48" s="1" t="s">
+      <c r="O48" s="9" t="s">
         <v>898</v>
       </c>
-      <c r="P48" s="1">
+      <c r="P48" s="9">
         <v>161</v>
       </c>
-      <c r="Q48" s="1">
+      <c r="Q48" s="9">
         <v>161</v>
       </c>
-      <c r="S48" s="1">
+      <c r="R48" s="9"/>
+      <c r="S48" s="9">
         <v>1</v>
       </c>
-      <c r="T48" s="1">
+      <c r="T48" s="9">
         <f>IF(L48="Wagon",(SQRT(SQRT(S48/27)))*10,IF(S48="","",SQRT(SQRT(S48/27))))</f>
         <v>4.3869133765083088</v>
       </c>
-      <c r="U48" s="14">
+      <c r="U48" s="28">
         <f t="shared" si="10"/>
         <v>47.923424608331878</v>
       </c>
-      <c r="V48" s="14">
+      <c r="V48" s="28">
         <f t="shared" si="11"/>
         <v>16.651228563089134</v>
       </c>
-      <c r="W48" s="20">
+      <c r="W48" s="30">
         <f t="shared" si="4"/>
         <v>4.9689440993788817E-2</v>
       </c>
-      <c r="X48" s="32">
+      <c r="X48" s="34">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -9189,7 +9202,7 @@
         <v>0</v>
       </c>
       <c r="U66" s="14" t="e">
-        <f t="shared" ref="U66:U97" si="16">IF(I66="","",(H66*SQRT(I66)*T66-(I66*2)+2)*0.985)</f>
+        <f t="shared" ref="U66:U92" si="16">IF(I66="","",(H66*SQRT(I66)*T66-(I66*2)+2)*0.985)</f>
         <v>#VALUE!</v>
       </c>
       <c r="V66" s="14" t="e">
@@ -34869,11 +34882,11 @@
         <v>2</v>
       </c>
       <c r="T445" s="1" t="str">
-        <f t="shared" ref="T445:T476" si="97">IF(L445="Wagon",(SQRT(SQRT(S445/27)))*10,IF(S445="","",SQRT(SQRT(S445/27))))</f>
+        <f t="shared" ref="T445" si="97">IF(L445="Wagon",(SQRT(SQRT(S445/27)))*10,IF(S445="","",SQRT(SQRT(S445/27))))</f>
         <v/>
       </c>
       <c r="U445" s="14" t="str">
-        <f t="shared" ref="U445:U476" si="98">IF(I445="","",(H445*SQRT(I445)*T445-(I445*2)+2)*0.985)</f>
+        <f t="shared" ref="U445" si="98">IF(I445="","",(H445*SQRT(I445)*T445-(I445*2)+2)*0.985)</f>
         <v/>
       </c>
       <c r="V445" s="14">
@@ -52803,7 +52816,7 @@
         <v/>
       </c>
       <c r="U832" s="14" t="str">
-        <f t="shared" ref="U832:U895" si="153">IF(I832="","",(H832*SQRT(I832)*T832-(I832*2)+2)*0.985)</f>
+        <f t="shared" ref="U832:U885" si="153">IF(I832="","",(H832*SQRT(I832)*T832-(I832*2)+2)*0.985)</f>
         <v/>
       </c>
       <c r="V832" s="14" t="str">
@@ -53547,7 +53560,7 @@
         <v/>
       </c>
       <c r="T854" s="1" t="str">
-        <f t="shared" ref="T854:T917" si="158">IF(L854="Wagon",(SQRT(SQRT(S854/27)))*10,IF(S854="","",SQRT(SQRT(S854/27))))</f>
+        <f t="shared" ref="T854:T885" si="158">IF(L854="Wagon",(SQRT(SQRT(S854/27)))*10,IF(S854="","",SQRT(SQRT(S854/27))))</f>
         <v/>
       </c>
       <c r="U854" s="14" t="str">

</xml_diff>

<commit_message>
Early Model for LNER Gresley Twin Third Brake
</commit_message>
<xml_diff>
--- a/docs/Cost Factor Calculator.xlsx
+++ b/docs/Cost Factor Calculator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BRTrains2-Extended\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4EC549D-B9AF-449A-8E1F-81CFB84E6C5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75504B9E-58EB-4639-ACD7-5EA50C4ADD84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cost Factor Calculator" sheetId="1" r:id="rId1"/>
@@ -5015,10 +5015,10 @@
   <dimension ref="A1:X884"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D179" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O22" sqref="O22"/>
+      <selection pane="bottomRight" activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5035,13 +5035,13 @@
     <col min="11" max="11" width="13" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.85546875" style="1" customWidth="1"/>
-    <col min="14" max="14" width="14.28515625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="11.140625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="3.85546875" style="1" customWidth="1"/>
+    <col min="15" max="15" width="6.85546875" style="1" customWidth="1"/>
     <col min="16" max="16" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="17.28515625" style="1" customWidth="1"/>
     <col min="18" max="18" width="20.42578125" style="1" customWidth="1"/>
     <col min="19" max="19" width="9.42578125" style="1" customWidth="1"/>
-    <col min="20" max="20" width="18" style="1" customWidth="1"/>
+    <col min="20" max="20" width="4.7109375" style="1" customWidth="1"/>
     <col min="21" max="21" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="23.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="18.7109375" style="1" customWidth="1"/>
@@ -11817,7 +11817,7 @@
         <v>0</v>
       </c>
       <c r="U98" s="14" t="e">
-        <f t="shared" ref="U98:U129" si="23">IF(I98="","",(H98*SQRT(I98)*T98-(I98*2)+2)*0.985)</f>
+        <f t="shared" ref="U98:U103" si="23">IF(I98="","",(H98*SQRT(I98)*T98-(I98*2)+2)*0.985)</f>
         <v>#VALUE!</v>
       </c>
       <c r="V98" s="14" t="e">
@@ -12057,7 +12057,7 @@
         <v>1177</v>
       </c>
       <c r="T102" s="1">
-        <f t="shared" ref="T102:T133" si="25">IF(L102="Wagon",(SQRT(SQRT(S102/27)))*10,IF(S102="","",SQRT(SQRT(S102/27))))</f>
+        <f t="shared" ref="T102:T103" si="25">IF(L102="Wagon",(SQRT(SQRT(S102/27)))*10,IF(S102="","",SQRT(SQRT(S102/27))))</f>
         <v>0</v>
       </c>
       <c r="U102" s="14" t="e">
@@ -17121,11 +17121,11 @@
         <v>2000</v>
       </c>
       <c r="T169" s="1">
-        <f t="shared" ref="T169:T200" si="40">IF(L169="Wagon",(SQRT(SQRT(S169/27)))*10,IF(S169="","",SQRT(SQRT(S169/27))))</f>
+        <f t="shared" ref="T169:T189" si="40">IF(L169="Wagon",(SQRT(SQRT(S169/27)))*10,IF(S169="","",SQRT(SQRT(S169/27))))</f>
         <v>2.9337057893113112</v>
       </c>
       <c r="U169" s="14">
-        <f t="shared" ref="U169:U200" si="41">IF(I169="","",(H169*SQRT(I169)*T169-(I169*2)+2)*0.985)</f>
+        <f t="shared" ref="U169:U197" si="41">IF(I169="","",(H169*SQRT(I169)*T169-(I169*2)+2)*0.985)</f>
         <v>80.114141691055707</v>
       </c>
       <c r="V169" s="14">
@@ -21400,7 +21400,7 @@
         <v>2000</v>
       </c>
       <c r="T225" s="1">
-        <f t="shared" ref="T225:T256" si="51">IF(L225="Wagon",(SQRT(SQRT(S225/27)))*10,IF(S225="","",SQRT(SQRT(S225/27))))</f>
+        <f t="shared" ref="T225:T251" si="51">IF(L225="Wagon",(SQRT(SQRT(S225/27)))*10,IF(S225="","",SQRT(SQRT(S225/27))))</f>
         <v>2.9337057893113112</v>
       </c>
       <c r="U225" s="14">
@@ -21852,7 +21852,7 @@
         <v>3.1564052529180788</v>
       </c>
       <c r="U231" s="14">
-        <f t="shared" ref="U231:U262" si="53">IF(I231="","",(H231*SQRT(I231)*T231-(I231*2)+2)*0.985)</f>
+        <f t="shared" ref="U231:U251" si="53">IF(I231="","",(H231*SQRT(I231)*T231-(I231*2)+2)*0.985)</f>
         <v>86.93356190879058</v>
       </c>
       <c r="V231" s="14">
@@ -29452,7 +29452,7 @@
         <v/>
       </c>
       <c r="U338" s="14" t="e">
-        <f t="shared" ref="U338:U369" si="81">IF(I338="","",(H338*SQRT(I338)*T338-(I338*2)+2)*0.985)</f>
+        <f t="shared" ref="U338:U359" si="81">IF(I338="","",(H338*SQRT(I338)*T338-(I338*2)+2)*0.985)</f>
         <v>#VALUE!</v>
       </c>
       <c r="V338" s="14">
@@ -41397,11 +41397,11 @@
         <v>1177</v>
       </c>
       <c r="T513" s="1" t="str">
-        <f t="shared" ref="T513:T544" si="118">IF(L513="Wagon",(SQRT(SQRT(S513/27)))*10,IF(S513="","",SQRT(SQRT(S513/27))))</f>
+        <f t="shared" ref="T513:T514" si="118">IF(L513="Wagon",(SQRT(SQRT(S513/27)))*10,IF(S513="","",SQRT(SQRT(S513/27))))</f>
         <v/>
       </c>
       <c r="U513" s="14" t="str">
-        <f t="shared" ref="U513:U544" si="119">IF(I513="","",(H513*SQRT(I513)*T513-(I513*2)+2)*0.985)</f>
+        <f t="shared" ref="U513:U514" si="119">IF(I513="","",(H513*SQRT(I513)*T513-(I513*2)+2)*0.985)</f>
         <v/>
       </c>
       <c r="V513" s="14" t="e">
@@ -58297,7 +58297,7 @@
         <v/>
       </c>
       <c r="U837" s="14" t="str">
-        <f t="shared" ref="U837:U900" si="164">IF(I837="","",(H837*SQRT(I837)*T837-(I837*2)+2)*0.985)</f>
+        <f t="shared" ref="U837:U884" si="164">IF(I837="","",(H837*SQRT(I837)*T837-(I837*2)+2)*0.985)</f>
         <v/>
       </c>
       <c r="V837" s="14" t="str">
@@ -59065,7 +59065,7 @@
         <v/>
       </c>
       <c r="T859" s="1" t="str">
-        <f t="shared" ref="T859:T922" si="170">IF(L859="Wagon",(SQRT(SQRT(S859/27)))*10,IF(S859="","",SQRT(SQRT(S859/27))))</f>
+        <f t="shared" ref="T859:T884" si="170">IF(L859="Wagon",(SQRT(SQRT(S859/27)))*10,IF(S859="","",SQRT(SQRT(S859/27))))</f>
         <v/>
       </c>
       <c r="U859" s="14" t="str">

</xml_diff>

<commit_message>
BR66 extra liveries and changes to the models.
</commit_message>
<xml_diff>
--- a/docs/Cost Factor Calculator.xlsx
+++ b/docs/Cost Factor Calculator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BRTrains2-Extended\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64E1835E-FC00-43B6-A1A5-46710CF03191}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83FD323E-400C-47FB-9DEF-1AA0070ADC3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{11AEBE64-33AB-4961-BAA4-7267ABB553C4}"/>
   </bookViews>
@@ -104,7 +104,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5197" uniqueCount="1737">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5199" uniqueCount="1737">
   <si>
     <t>ITEM_NAME</t>
   </si>
@@ -6932,7 +6932,7 @@
   <dimension ref="A1:Y939"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="P42" sqref="P42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11126,7 +11126,9 @@
         <f t="shared" si="13"/>
         <v>1</v>
       </c>
-      <c r="O54" s="1"/>
+      <c r="O54" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="P54" s="1" t="s">
         <v>1134</v>
       </c>
@@ -11281,6 +11283,9 @@
         <f t="shared" si="13"/>
         <v>1</v>
       </c>
+      <c r="O56" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="R56" s="1">
         <v>128</v>
       </c>
@@ -16307,7 +16312,7 @@
         <v>1134</v>
       </c>
       <c r="T130" s="1">
-        <f t="shared" ref="T130:T161" si="29">IF(L130="Wagon",(SQRT(SQRT(S130/27)))*10,IF(S130="","",SQRT(SQRT(S130/27))))</f>
+        <f t="shared" ref="T130" si="29">IF(L130="Wagon",(SQRT(SQRT(S130/27)))*10,IF(S130="","",SQRT(SQRT(S130/27))))</f>
         <v>0</v>
       </c>
       <c r="U130" s="13" t="e">
@@ -30595,7 +30600,7 @@
         <v>2.2564908092374663</v>
       </c>
       <c r="U322" s="13">
-        <f t="shared" ref="U322:U385" si="63">IF(I322="","",(H322*SQRT(I322)*T322-(I322*2)+2)*0.985)</f>
+        <f t="shared" ref="U322:U340" si="63">IF(I322="","",(H322*SQRT(I322)*T322-(I322*2)+2)*0.985)</f>
         <v>43.988221632013868</v>
       </c>
       <c r="V322" s="13">
@@ -30744,7 +30749,7 @@
         <v>700</v>
       </c>
       <c r="T324" s="1">
-        <f t="shared" ref="T324:T387" si="66">IF(L324="Wagon",(SQRT(SQRT(S324/27)))*10,IF(S324="","",SQRT(SQRT(S324/27))))</f>
+        <f t="shared" ref="T324:T363" si="66">IF(L324="Wagon",(SQRT(SQRT(S324/27)))*10,IF(S324="","",SQRT(SQRT(S324/27))))</f>
         <v>2.2564908092374663</v>
       </c>
       <c r="U324" s="13">
@@ -34806,10 +34811,10 @@
         <v>23</v>
       </c>
       <c r="P378" s="38">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="Q378" s="38">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="R378" s="38">
         <v>247</v>
@@ -34827,11 +34832,11 @@
       </c>
       <c r="V378" s="44">
         <f t="shared" si="75"/>
-        <v>23.298903129508759</v>
+        <v>23.834580075293811</v>
       </c>
       <c r="W378" s="39">
         <f t="shared" si="76"/>
-        <v>9.3023255813953487E-2</v>
+        <v>8.8888888888888892E-2</v>
       </c>
       <c r="X378" s="40">
         <f t="shared" si="77"/>
@@ -35264,10 +35269,10 @@
         <v>23</v>
       </c>
       <c r="P385" s="38">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="Q385" s="38">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="R385" s="38">
         <v>247</v>
@@ -35285,11 +35290,11 @@
       </c>
       <c r="V385" s="44">
         <f t="shared" si="75"/>
-        <v>23.298903129508759</v>
+        <v>23.834580075293811</v>
       </c>
       <c r="W385" s="39">
         <f t="shared" si="76"/>
-        <v>9.3023255813953487E-2</v>
+        <v>8.8888888888888892E-2</v>
       </c>
       <c r="X385" s="40">
         <f t="shared" si="77"/>
@@ -35327,7 +35332,7 @@
         <v>1</v>
       </c>
       <c r="J386" s="38">
-        <v>122</v>
+        <v>102</v>
       </c>
       <c r="K386" s="38">
         <v>0</v>
@@ -35346,10 +35351,10 @@
         <v>23</v>
       </c>
       <c r="P386" s="38">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="Q386" s="38">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="R386" s="38">
         <v>247</v>
@@ -35367,15 +35372,15 @@
       </c>
       <c r="V386" s="44">
         <f t="shared" si="75"/>
-        <v>24.57599290850321</v>
+        <v>23.834580075293811</v>
       </c>
       <c r="W386" s="39">
         <f t="shared" si="76"/>
-        <v>0.1</v>
+        <v>8.8888888888888892E-2</v>
       </c>
       <c r="X386" s="40">
         <f t="shared" si="77"/>
-        <v>0.2024590163934426</v>
+        <v>0.24215686274509804</v>
       </c>
     </row>
     <row r="387" spans="1:25" s="48" customFormat="1" x14ac:dyDescent="0.25">
@@ -38165,11 +38170,11 @@
         <v>4480</v>
       </c>
       <c r="T428" s="1">
-        <f t="shared" ref="T428:T459" si="87">IF(L428="Wagon",(SQRT(SQRT(S428/27)))*10,IF(S428="","",SQRT(SQRT(S428/27))))</f>
+        <f t="shared" ref="T428:T451" si="87">IF(L428="Wagon",(SQRT(SQRT(S428/27)))*10,IF(S428="","",SQRT(SQRT(S428/27))))</f>
         <v>3.5890421806368633</v>
       </c>
       <c r="U428" s="13">
-        <f t="shared" ref="U428:U459" si="88">IF(I428="","",(H428*SQRT(I428)*T428-(I428*2)+2)*0.985)</f>
+        <f t="shared" ref="U428:U456" si="88">IF(I428="","",(H428*SQRT(I428)*T428-(I428*2)+2)*0.985)</f>
         <v>106.65101405330265</v>
       </c>
       <c r="V428" s="13">
@@ -49804,7 +49809,7 @@
         <v/>
       </c>
       <c r="U582" s="13" t="e">
-        <f t="shared" ref="U582:U613" si="120">IF(I582="","",(H582*SQRT(I582)*T582-(I582*2)+2)*0.985)</f>
+        <f t="shared" ref="U582:U602" si="120">IF(I582="","",(H582*SQRT(I582)*T582-(I582*2)+2)*0.985)</f>
         <v>#VALUE!</v>
       </c>
       <c r="V582" s="13" t="e">
@@ -73318,11 +73323,11 @@
     </row>
     <row r="928" spans="4:24" x14ac:dyDescent="0.25">
       <c r="T928" s="1" t="str">
-        <f t="shared" ref="T928:T991" si="175">IF(L928="Wagon",(SQRT(SQRT(S928/27)))*10,IF(S928="","",SQRT(SQRT(S928/27))))</f>
+        <f t="shared" ref="T928:T939" si="175">IF(L928="Wagon",(SQRT(SQRT(S928/27)))*10,IF(S928="","",SQRT(SQRT(S928/27))))</f>
         <v/>
       </c>
       <c r="U928" s="13" t="str">
-        <f t="shared" ref="U928:U991" si="176">IF(I928="","",(H928*SQRT(I928)*T928-(I928*2)+2)*0.985)</f>
+        <f t="shared" ref="U928:U939" si="176">IF(I928="","",(H928*SQRT(I928)*T928-(I928*2)+2)*0.985)</f>
         <v/>
       </c>
       <c r="V928" s="13" t="str">

</xml_diff>

<commit_message>
LNER Gresley Twin BT-T Nearly completed. Loading Sprites needed.
</commit_message>
<xml_diff>
--- a/docs/Cost Factor Calculator.xlsx
+++ b/docs/Cost Factor Calculator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BRTrains2-Extended\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33FE8407-B063-4535-A0E2-EA822B65BDE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B105391-79FD-4A0A-B278-6B8D929EABF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{11AEBE64-33AB-4961-BAA4-7267ABB553C4}"/>
   </bookViews>
@@ -6051,174 +6051,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF9966FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7C80"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9966FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9933FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF488FD0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF456A2C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7ABC32"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF456A2C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFF5050"/>
         </patternFill>
       </fill>
@@ -6360,6 +6192,174 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF456A2C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7C80"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF9966FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF9933FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF9966FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF488FD0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF456A2C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7ABC32"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF456A2C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -7224,8 +7224,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A201" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F229" sqref="F229"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19378,7 +19378,7 @@
         <v>4.3869133765083088</v>
       </c>
       <c r="U191" s="13">
-        <f t="shared" ref="U191:U222" si="39">IF(I191="","",(H191*SQRT(I191)*T191-(I191*2)+2)*0.985)</f>
+        <f t="shared" ref="U191:U206" si="39">IF(I191="","",(H191*SQRT(I191)*T191-(I191*2)+2)*0.985)</f>
         <v>0</v>
       </c>
       <c r="V191" s="13">
@@ -21779,82 +21779,82 @@
       <c r="Y232" s="12"/>
       <c r="Z232" s="12"/>
     </row>
-    <row r="233" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A233" s="22">
+    <row r="233" spans="1:26" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A233" s="20">
         <v>901</v>
       </c>
-      <c r="B233" s="9" t="s">
+      <c r="B233" s="6" t="s">
         <v>1121</v>
       </c>
-      <c r="C233" s="9" t="s">
+      <c r="C233" s="6" t="s">
         <v>1122</v>
       </c>
-      <c r="D233" s="1" t="str">
+      <c r="D233" s="6" t="str">
         <f t="shared" si="63"/>
         <v>LN</v>
       </c>
-      <c r="E233" s="9" t="s">
+      <c r="E233" s="6" t="s">
         <v>349</v>
       </c>
-      <c r="F233" s="23">
+      <c r="F233" s="7">
         <v>1940</v>
       </c>
-      <c r="G233" s="23"/>
-      <c r="H233" s="9">
+      <c r="G233" s="7"/>
+      <c r="H233" s="6">
         <f t="shared" si="64"/>
         <v>10.583005244258363</v>
       </c>
-      <c r="I233" s="9">
+      <c r="I233" s="6">
         <v>2</v>
       </c>
-      <c r="J233" s="9">
+      <c r="J233" s="6">
         <v>47</v>
       </c>
-      <c r="K233" s="9">
+      <c r="K233" s="6">
         <v>140</v>
       </c>
-      <c r="L233" s="9" t="s">
+      <c r="L233" s="6" t="s">
         <v>331</v>
       </c>
-      <c r="M233" s="9" t="s">
+      <c r="M233" s="6" t="s">
         <v>331</v>
       </c>
-      <c r="N233" s="9" t="str">
+      <c r="N233" s="6" t="str">
         <f t="shared" si="65"/>
         <v/>
       </c>
-      <c r="O233" s="9" t="s">
+      <c r="O233" s="6" t="s">
         <v>835</v>
       </c>
-      <c r="P233" s="9">
+      <c r="P233" s="6">
         <v>60</v>
       </c>
-      <c r="Q233" s="9">
+      <c r="Q233" s="6">
         <v>60</v>
       </c>
-      <c r="R233" s="9">
-        <v>0</v>
-      </c>
-      <c r="S233" s="9">
+      <c r="R233" s="6">
+        <v>0</v>
+      </c>
+      <c r="S233" s="6">
         <v>1</v>
       </c>
-      <c r="T233" s="15">
+      <c r="T233" s="35">
         <f t="shared" si="46"/>
         <v>4.3869133765083088</v>
       </c>
-      <c r="U233" s="23">
+      <c r="U233" s="7">
         <f t="shared" si="62"/>
         <v>62.702447750977925</v>
       </c>
-      <c r="V233" s="23">
+      <c r="V233" s="7">
         <f t="shared" si="58"/>
         <v>16.265765616977859</v>
       </c>
-      <c r="W233" s="25">
+      <c r="W233" s="26">
         <f t="shared" si="59"/>
         <v>0.13333333333333333</v>
       </c>
-      <c r="X233" s="29">
+      <c r="X233" s="28">
         <f t="shared" si="60"/>
         <v>0</v>
       </c>
@@ -35679,7 +35679,7 @@
         <v>2.7596690210718946</v>
       </c>
       <c r="U410" s="13">
-        <f t="shared" ref="U410:U473" si="96">IF(I410="","",(H410*SQRT(I410)*T410-(I410*2)+2)*0.985)</f>
+        <f t="shared" ref="U410:U428" si="96">IF(I410="","",(H410*SQRT(I410)*T410-(I410*2)+2)*0.985)</f>
         <v>56.354233746895815</v>
       </c>
       <c r="V410" s="13">
@@ -41644,7 +41644,7 @@
         <v/>
       </c>
       <c r="U493" s="47" t="str">
-        <f t="shared" ref="U493:U524" si="115">IF(I493="","",(H493*SQRT(I493)*T493-(I493*2)+2)*0.985)</f>
+        <f t="shared" ref="U493:U522" si="115">IF(I493="","",(H493*SQRT(I493)*T493-(I493*2)+2)*0.985)</f>
         <v/>
       </c>
       <c r="V493" s="47" t="str">
@@ -53671,7 +53671,7 @@
         <v/>
       </c>
       <c r="U649" s="13" t="e">
-        <f t="shared" ref="U649:U680" si="147">IF(I649="","",(H649*SQRT(I649)*T649-(I649*2)+2)*0.985)</f>
+        <f t="shared" ref="U649:U676" si="147">IF(I649="","",(H649*SQRT(I649)*T649-(I649*2)+2)*0.985)</f>
         <v>#VALUE!</v>
       </c>
       <c r="V649" s="13">
@@ -73996,7 +73996,7 @@
         <v>2.074443257628261</v>
       </c>
       <c r="U938" s="13">
-        <f t="shared" ref="U938:U1001" si="190">IF(I938="","",(H938*SQRT(I938)*T938-(I938*2)+2)*0.985)</f>
+        <f t="shared" ref="U938:U997" si="190">IF(I938="","",(H938*SQRT(I938)*T938-(I938*2)+2)*0.985)</f>
         <v>33.49550303707462</v>
       </c>
       <c r="V938" s="13" t="e">
@@ -77869,81 +77869,81 @@
     <sortCondition ref="C2:C869"/>
   </sortState>
   <conditionalFormatting sqref="D1:D9982">
-    <cfRule type="cellIs" dxfId="23" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="2" operator="equal">
       <formula>"Re"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="4" operator="containsText" text="GC">
+    <cfRule type="containsText" dxfId="43" priority="4" operator="containsText" text="GC">
       <formula>NOT(ISERROR(SEARCH("GC",D1)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="5" operator="equal">
       <formula>"GE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="6" operator="equal">
       <formula>"LM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="7" operator="equal">
       <formula>"MR"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="8" operator="equal">
       <formula>"SD"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="9" operator="equal">
       <formula>"SE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="10" operator="equal">
       <formula>"GN"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="11" operator="equal">
       <formula>"SR"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="12" operator="containsText" text="LN">
+    <cfRule type="containsText" dxfId="35" priority="12" operator="containsText" text="LN">
       <formula>NOT(ISERROR(SEARCH("LN",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="GW">
+    <cfRule type="containsText" dxfId="34" priority="14" operator="containsText" text="GW">
       <formula>NOT(ISERROR(SEARCH("GW",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="15" operator="containsText" text="BR">
+    <cfRule type="containsText" dxfId="33" priority="15" operator="containsText" text="BR">
       <formula>NOT(ISERROR(SEARCH("BR",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="L1:M1048561">
+    <cfRule type="cellIs" dxfId="32" priority="3" operator="equal">
+      <formula>"Gas"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="L2:M209 L211:M1048561">
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="1" operator="equal">
       <formula>"15OH"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="17" operator="equal">
       <formula>"4RAIL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="18" operator="equal">
       <formula>"Dual"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="19" operator="equal">
       <formula>"OHLE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="20" operator="equal">
       <formula>"3RAIL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="21" operator="equal">
       <formula>"Gas Turbine"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="22" operator="equal">
       <formula>"Diesel-Electric"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="23" operator="equal">
       <formula>"Wagon"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="24" operator="equal">
       <formula>"Steam"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="25" operator="equal">
       <formula>"Electric"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="26" operator="equal">
       <formula>"Diesel"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L1:M1048561">
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
-      <formula>"Gas"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -78554,69 +78554,69 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D2">
-    <cfRule type="containsText" dxfId="44" priority="1" operator="containsText" text="GC">
+    <cfRule type="containsText" dxfId="20" priority="1" operator="containsText" text="GC">
       <formula>NOT(ISERROR(SEARCH("GC",D2)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="2" operator="equal">
       <formula>"GE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="3" operator="equal">
       <formula>"LM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="4" operator="equal">
       <formula>"MR"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="5" operator="equal">
       <formula>"SD"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="6" operator="equal">
       <formula>"SE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="7" operator="equal">
       <formula>"GN"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="8" operator="equal">
       <formula>"SR"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="9" operator="containsText" text="LN">
+    <cfRule type="containsText" dxfId="12" priority="9" operator="containsText" text="LN">
       <formula>NOT(ISERROR(SEARCH("LN",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="35" priority="10" operator="containsText" text="GW">
+    <cfRule type="containsText" dxfId="11" priority="10" operator="containsText" text="GW">
       <formula>NOT(ISERROR(SEARCH("GW",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="11" operator="containsText" text="BR">
+    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="BR">
       <formula>NOT(ISERROR(SEARCH("BR",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:M2">
-    <cfRule type="cellIs" dxfId="33" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="12" operator="equal">
       <formula>"4RAIL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="13" operator="equal">
       <formula>"Dual"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="14" operator="equal">
       <formula>"OHLE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="15" operator="equal">
       <formula>"3RAIL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="16" operator="equal">
       <formula>"Gas Turbine"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="17" operator="equal">
       <formula>"Diesel-Electric"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="18" operator="equal">
       <formula>"Wagon"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="19" operator="equal">
       <formula>"Steam"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="20" operator="equal">
       <formula>"Electric"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="21" operator="equal">
       <formula>"Diesel"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Gresley Twin BT-T Completed. Need to realign 108 reversed view.
</commit_message>
<xml_diff>
--- a/docs/Cost Factor Calculator.xlsx
+++ b/docs/Cost Factor Calculator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BRTrains2-Extended\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B105391-79FD-4A0A-B278-6B8D929EABF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{461FDD64-703B-4715-A6D4-06224506D02B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{11AEBE64-33AB-4961-BAA4-7267ABB553C4}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{11AEBE64-33AB-4961-BAA4-7267ABB553C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Cost Factor Calculator" sheetId="1" r:id="rId1"/>
@@ -7224,8 +7224,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A201" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F229" sqref="F229"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7237,7 +7237,7 @@
     <col min="5" max="5" width="8.42578125" style="1" customWidth="1"/>
     <col min="6" max="6" width="9.85546875" style="13" customWidth="1"/>
     <col min="7" max="7" width="10.5703125" style="13" customWidth="1"/>
-    <col min="8" max="8" width="2" style="1" customWidth="1"/>
+    <col min="8" max="8" width="6" style="1" customWidth="1"/>
     <col min="9" max="9" width="11.85546875" style="1" customWidth="1"/>
     <col min="10" max="10" width="12.7109375" style="1" customWidth="1"/>
     <col min="11" max="11" width="13" style="1" bestFit="1" customWidth="1"/>
@@ -21800,7 +21800,7 @@
         <v>1940</v>
       </c>
       <c r="G233" s="7"/>
-      <c r="H233" s="6">
+      <c r="H233" s="1">
         <f t="shared" si="64"/>
         <v>10.583005244258363</v>
       </c>
@@ -21843,7 +21843,7 @@
         <v>4.3869133765083088</v>
       </c>
       <c r="U233" s="7">
-        <f t="shared" si="62"/>
+        <f>IF(I233="","",(H233*SQRT(I233)*T233-(I233*2)+2)*0.985)</f>
         <v>62.702447750977925</v>
       </c>
       <c r="V233" s="7">

</xml_diff>